<commit_message>
atualizado arquivo excel transporte
</commit_message>
<xml_diff>
--- a/aula_10/exemplo.xlsx
+++ b/aula_10/exemplo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acsjunior/Documents/Projects/pyomo-lessons/aula_10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6D0D5C-D058-AE4B-BF05-693DB1018DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DD026C-E066-1F4D-8D57-80562117F998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{B51FCA0A-6C63-3F41-A35C-8C8C5C7691D3}"/>
+    <workbookView xWindow="-6660" yWindow="-21100" windowWidth="38360" windowHeight="21100" xr2:uid="{B51FCA0A-6C63-3F41-A35C-8C8C5C7691D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
   <si>
     <t>Osasco</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Custo total</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -579,203 +582,318 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34A03B10-9545-E54E-9E76-CCECA71566B0}">
-  <dimension ref="B3:F18"/>
+  <dimension ref="I3:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="12.5" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="J3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="6"/>
-      <c r="C4" s="12" t="s">
+      <c r="K3" s="10"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I4" s="6"/>
+      <c r="J4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="K4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="L4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="M4" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="7" t="s">
+    <row r="5" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="16">
+      <c r="J5" s="16">
         <v>12</v>
       </c>
-      <c r="D5" s="16">
+      <c r="K5" s="16">
         <v>22</v>
       </c>
-      <c r="E5" s="16">
+      <c r="L5" s="16">
         <v>30</v>
       </c>
-      <c r="F5" s="4">
+      <c r="M5" s="4">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="s">
+    <row r="6" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="16">
+      <c r="J6" s="16">
         <v>18</v>
       </c>
-      <c r="D6" s="16">
+      <c r="K6" s="16">
         <v>24</v>
       </c>
-      <c r="E6" s="16">
+      <c r="L6" s="16">
         <v>32</v>
       </c>
-      <c r="F6" s="4">
+      <c r="M6" s="4">
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="s">
+    <row r="7" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="16">
+      <c r="J7" s="16">
         <v>22</v>
       </c>
-      <c r="D7" s="16">
+      <c r="K7" s="16">
         <v>15</v>
       </c>
-      <c r="E7" s="16">
+      <c r="L7" s="16">
         <v>34</v>
       </c>
-      <c r="F7" s="14">
+      <c r="M7" s="14">
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="8" t="s">
+    <row r="8" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3">
+      <c r="J8" s="3">
         <v>120</v>
       </c>
-      <c r="D8" s="3">
+      <c r="K8" s="3">
         <v>130</v>
       </c>
-      <c r="E8" s="15">
+      <c r="L8" s="15">
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="5" t="s">
+    <row r="11" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="J11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="6"/>
-      <c r="C12" s="12" t="s">
+      <c r="K11" s="10"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I12" s="6"/>
+      <c r="J12" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="K12" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="L12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="M12" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="7" t="s">
+    <row r="13" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I13" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="4">
-        <f>SUM(C13:E13)</f>
+      <c r="J13" s="1">
+        <v>100</v>
+      </c>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="4">
+        <f>SUM(J13:L13)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1">
+        <v>140</v>
+      </c>
+      <c r="M14" s="4">
+        <f t="shared" ref="M14:M15" si="0">SUM(J14:L14)</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" s="1">
+        <v>20</v>
+      </c>
+      <c r="K15" s="1">
+        <v>130</v>
+      </c>
+      <c r="L15" s="1">
+        <v>10</v>
+      </c>
+      <c r="M15" s="14">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I16" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="3">
+        <f>SUM(J13:J15)</f>
+        <v>120</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" ref="K16:L16" si="1">SUM(K13:K15)</f>
+        <v>130</v>
+      </c>
+      <c r="L16" s="15">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I18" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="18">
+        <f>SUMPRODUCT(J13:L15,J5:L7)</f>
+        <v>8410</v>
+      </c>
+    </row>
+    <row r="21" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K21" s="10"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I22" s="6"/>
+      <c r="J22" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K22" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="M22" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I23" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="7" t="s">
+      <c r="J23" s="1">
+        <v>100</v>
+      </c>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="4">
+        <f>SUM(J23:L23)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I24" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="4">
-        <f t="shared" ref="F14:F15" si="0">SUM(C14:E14)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="7" t="s">
+      <c r="J24" s="1">
+        <v>20</v>
+      </c>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1">
+        <v>120</v>
+      </c>
+      <c r="M24" s="4">
+        <f t="shared" ref="M24:M25" si="2">SUM(J24:L24)</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I25" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="8" t="s">
+      <c r="J25" s="1"/>
+      <c r="K25" s="1">
+        <v>130</v>
+      </c>
+      <c r="L25" s="1">
+        <v>30</v>
+      </c>
+      <c r="M25" s="14">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I26" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="3">
-        <f>SUM(C13:C15)</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="3">
-        <f t="shared" ref="D16:E16" si="1">SUM(D13:D15)</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="17" t="s">
+      <c r="J26" s="3">
+        <f>SUM(J23:J25)</f>
+        <v>120</v>
+      </c>
+      <c r="K26" s="3">
+        <f t="shared" ref="K26" si="3">SUM(K23:K25)</f>
+        <v>130</v>
+      </c>
+      <c r="L26" s="15">
+        <f t="shared" ref="L26" si="4">SUM(L23:L25)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I28" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="18">
-        <f>SUMPRODUCT(C13:E15,C5:E7)</f>
-        <v>0</v>
+      <c r="J28" s="18">
+        <f>SUMPRODUCT(J23:L25,J5:L7)</f>
+        <v>8370</v>
+      </c>
+    </row>
+    <row r="31" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="L31" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:E11"/>
+  <mergeCells count="6">
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="J21:L21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>